<commit_message>
Updated reporting and addressed inconsistencies in side-data
</commit_message>
<xml_diff>
--- a/tabular/eve/efv-refseq-locus-data.xlsx
+++ b/tabular/eve/efv-refseq-locus-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/RNA+ve/Flaviviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6439CB-D6DC-1943-A2AD-8F27F3B063FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CEE66FB-F1DF-E94D-8A9E-59F257882720}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="1460" windowWidth="27280" windowHeight="9820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -664,13 +664,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="101" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>